<commit_message>
align CM changes with main data and new get_data()
</commit_message>
<xml_diff>
--- a/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
+++ b/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/case_studies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\models_extra\CM_module\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EA9594-653A-7E4B-A44B-503E8F484CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414AB2C-945D-4D21-A497-A4C4F728A685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="52" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="44" activeTab="49" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="CompletionsPads" sheetId="3" r:id="rId6"/>
     <sheet name="SWDSites" sheetId="4" r:id="rId7"/>
     <sheet name="WaterQualityComponents" sheetId="125" r:id="rId8"/>
-    <sheet name="FreshwaterSources" sheetId="35" r:id="rId9"/>
+    <sheet name="ExternalWaterSources" sheetId="35" r:id="rId9"/>
     <sheet name="StorageSites" sheetId="36" r:id="rId10"/>
     <sheet name="TreatmentSites" sheetId="37" r:id="rId11"/>
     <sheet name="NetworkNodes" sheetId="39" r:id="rId12"/>
@@ -54,15 +54,15 @@
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId39"/>
     <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId40"/>
     <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId41"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId42"/>
+    <sheet name="ExtWaterSourcingAvailability" sheetId="47" r:id="rId42"/>
     <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId43"/>
     <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId44"/>
     <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId45"/>
     <sheet name="StorageCost" sheetId="119" r:id="rId46"/>
     <sheet name="StorageWithdrawalRevenue" sheetId="120" r:id="rId47"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId48"/>
+    <sheet name="ExternalSourcingCost" sheetId="52" r:id="rId48"/>
     <sheet name="BeneficialReuseCost" sheetId="123" r:id="rId49"/>
-    <sheet name="BeneficialReuseRevenue" sheetId="124" r:id="rId50"/>
+    <sheet name="BeneficialReuseCredit" sheetId="124" r:id="rId50"/>
     <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId51"/>
     <sheet name="TruckingTime" sheetId="7" r:id="rId52"/>
     <sheet name="TreatmentEfficiency" sheetId="107" r:id="rId53"/>
@@ -2121,15 +2121,15 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.5" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2141,7 +2141,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="14"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="15"/>
       <c r="C3" s="16" t="s">
         <v>0</v>
@@ -2155,7 +2155,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -2167,7 +2167,7 @@
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="17" t="s">
         <v>1</v>
@@ -2181,7 +2181,7 @@
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
         <v>2</v>
@@ -2195,7 +2195,7 @@
       <c r="J6" s="17"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
         <v>3</v>
@@ -2209,7 +2209,7 @@
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="15"/>
       <c r="C8" s="17" t="s">
         <v>4</v>
@@ -2223,7 +2223,7 @@
       <c r="J8" s="17"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="s">
         <v>5</v>
@@ -2237,7 +2237,7 @@
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
       <c r="C10" s="17" t="s">
         <v>6</v>
@@ -2251,7 +2251,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="18"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -2263,7 +2263,7 @@
       <c r="J11" s="17"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="15"/>
       <c r="C12" s="17" t="s">
         <v>7</v>
@@ -2277,7 +2277,7 @@
       <c r="J12" s="17"/>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="C13" s="17" t="s">
         <v>8</v>
@@ -2291,7 +2291,7 @@
       <c r="J13" s="17"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2303,7 +2303,7 @@
       <c r="J14" s="17"/>
       <c r="K14" s="18"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
       <c r="C15" s="17" t="s">
         <v>9</v>
@@ -2317,7 +2317,7 @@
       <c r="J15" s="17"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
       <c r="C16" s="17" t="s">
         <v>10</v>
@@ -2331,7 +2331,7 @@
       <c r="J16" s="17"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="17" t="s">
         <v>11</v>
@@ -2345,7 +2345,7 @@
       <c r="J17" s="17"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="17" t="s">
         <v>12</v>
@@ -2359,7 +2359,7 @@
       <c r="J18" s="17"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -2371,7 +2371,7 @@
       <c r="J19" s="17"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -2383,7 +2383,7 @@
       <c r="J20" s="17"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="C21" s="19" t="s">
         <v>13</v>
@@ -2399,7 +2399,7 @@
       <c r="J21" s="17"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -2411,7 +2411,7 @@
       <c r="J22" s="17"/>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="15"/>
       <c r="C23" s="20" t="s">
         <v>15</v>
@@ -2427,7 +2427,7 @@
       <c r="J23" s="17"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
       <c r="C24" s="20" t="s">
         <v>17</v>
@@ -2443,7 +2443,7 @@
       <c r="J24" s="17"/>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="15"/>
       <c r="C25" s="20" t="s">
         <v>19</v>
@@ -2459,7 +2459,7 @@
       <c r="J25" s="17"/>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="15"/>
       <c r="C26" s="20" t="s">
         <v>21</v>
@@ -2475,7 +2475,7 @@
       <c r="J26" s="17"/>
       <c r="K26" s="18"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="15"/>
       <c r="C27" s="20" t="s">
         <v>23</v>
@@ -2491,7 +2491,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="15"/>
       <c r="C28" s="20" t="s">
         <v>25</v>
@@ -2507,7 +2507,7 @@
       <c r="J28" s="17"/>
       <c r="K28" s="18"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="15"/>
       <c r="C29" s="20" t="s">
         <v>27</v>
@@ -2523,7 +2523,7 @@
       <c r="J29" s="17"/>
       <c r="K29" s="18"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="15"/>
       <c r="C30" s="20" t="s">
         <v>29</v>
@@ -2539,7 +2539,7 @@
       <c r="J30" s="17"/>
       <c r="K30" s="18"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="15"/>
       <c r="C31" s="20" t="s">
         <v>31</v>
@@ -2558,7 +2558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="15"/>
       <c r="C32" s="20" t="s">
         <v>34</v>
@@ -2574,7 +2574,7 @@
       <c r="J32" s="17"/>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="15"/>
       <c r="C33" s="20" t="s">
         <v>36</v>
@@ -2590,7 +2590,7 @@
       <c r="J33" s="17"/>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="15"/>
       <c r="C34" s="20" t="s">
         <v>38</v>
@@ -2606,7 +2606,7 @@
       <c r="J34" s="17"/>
       <c r="K34" s="18"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="15"/>
       <c r="C35" s="20" t="s">
         <v>40</v>
@@ -2622,7 +2622,7 @@
       <c r="J35" s="17"/>
       <c r="K35" s="18"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="15"/>
       <c r="C36" s="20" t="s">
         <v>42</v>
@@ -2638,7 +2638,7 @@
       <c r="J36" s="17"/>
       <c r="K36" s="18"/>
     </row>
-    <row r="37" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
@@ -2681,36 +2681,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="3.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" style="1"/>
+    <col min="6" max="13" width="9.109375" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="11.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
     </row>
   </sheetData>
@@ -2728,30 +2728,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="3.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" style="1"/>
+    <col min="6" max="13" width="9.109375" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="11.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
@@ -2759,16 +2759,16 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
     </row>
   </sheetData>
@@ -2787,30 +2787,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="3.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" style="1"/>
+    <col min="6" max="13" width="9.109375" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="11.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
@@ -2818,99 +2818,99 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
     </row>
   </sheetData>
@@ -2929,18 +2929,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>134</v>
       </c>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -3005,7 +3005,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>92</v>
       </c>
@@ -3053,18 +3053,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -3130,18 +3130,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -3170,18 +3170,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>139</v>
       </c>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>125</v>
       </c>
@@ -3250,7 +3250,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
@@ -3268,7 +3268,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>127</v>
       </c>
@@ -3286,7 +3286,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>128</v>
       </c>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="J7" s="28"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>129</v>
       </c>
@@ -3323,7 +3323,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>130</v>
       </c>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>132</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3409,18 +3409,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>139</v>
       </c>
@@ -3428,61 +3428,61 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="28"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B6" s="28"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B7" s="28"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="28"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="28"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="28"/>
     </row>
-    <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B11" s="9"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
     </row>
@@ -3501,18 +3501,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>139</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
@@ -3532,21 +3532,21 @@
       </c>
       <c r="C3" s="28"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="28"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="28"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>127</v>
       </c>
@@ -3555,42 +3555,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="28"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="28"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="28"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="28"/>
     </row>
-    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3611,18 +3611,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>139</v>
       </c>
@@ -3633,21 +3633,21 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="28"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="28"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
@@ -3656,42 +3656,42 @@
       </c>
       <c r="C5" s="28"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="28"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="28"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="28"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="28"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="28"/>
     </row>
-    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>132</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3723,61 +3723,61 @@
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.5" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C3" s="37"/>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C21" s="38"/>
       <c r="F21" s="38"/>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C23" s="39"/>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C24" s="39"/>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C25" s="39"/>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C26" s="39"/>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C27" s="39"/>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C28" s="39"/>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C29" s="39"/>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C30" s="39"/>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C31" s="39"/>
       <c r="M31" s="24"/>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C32" s="39"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="39"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="39"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="39"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="39"/>
     </row>
   </sheetData>
@@ -3795,18 +3795,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>139</v>
       </c>
@@ -3814,55 +3814,55 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="80"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="80"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="80"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B6" s="80"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B7" s="80"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="80"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B9" s="80"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="80"/>
     </row>
-    <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>132</v>
       </c>
@@ -3885,18 +3885,18 @@
       <selection sqref="A1:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="13.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>117</v>
       </c>
@@ -3957,18 +3957,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>146</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>114</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>115</v>
       </c>
@@ -4010,9 +4010,9 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>228</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>114</v>
       </c>
@@ -4074,7 +4074,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>115</v>
       </c>
@@ -4106,18 +4106,18 @@
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -4125,13 +4125,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
@@ -4153,18 +4153,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -4172,13 +4172,13 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
@@ -4200,17 +4200,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>117</v>
       </c>
@@ -4240,18 +4240,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
@@ -4326,18 +4326,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>134</v>
       </c>
@@ -4345,25 +4345,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="28"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B5" s="28"/>
     </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>92</v>
       </c>
@@ -4385,18 +4385,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="19.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>146</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>114</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>115</v>
       </c>
@@ -4437,33 +4437,33 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="92.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="92.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="48" width="9.1640625" style="1"/>
-    <col min="49" max="49" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.1640625" style="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.109375" style="1"/>
+    <col min="49" max="49" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="J2" s="59"/>
       <c r="K2" s="61"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>49</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>56</v>
       </c>
@@ -4537,7 +4537,7 @@
       <c r="J4" s="49"/>
       <c r="K4" s="51"/>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>61</v>
       </c>
@@ -4555,7 +4555,7 @@
       <c r="J5" s="50"/>
       <c r="K5" s="52"/>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>64</v>
       </c>
@@ -4579,7 +4579,7 @@
       <c r="J6" s="50"/>
       <c r="K6" s="52"/>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>68</v>
       </c>
@@ -4603,7 +4603,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="52"/>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>73</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
         <v>77</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AT10" s="1" t="s">
         <v>54</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AU11" s="1" t="s">
         <v>87</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AU12" s="1" t="s">
         <v>59</v>
       </c>
@@ -4773,18 +4773,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>134</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>92</v>
       </c>
@@ -4854,18 +4854,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="18.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -4902,18 +4902,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -4944,18 +4944,18 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -4986,24 +4986,24 @@
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="53" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="53" width="9.109375" style="1"/>
     <col min="54" max="54" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="16384" width="9.1640625" style="1"/>
+    <col min="55" max="55" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -5327,10 +5327,10 @@
       <c r="BB3" s="71"/>
       <c r="BC3" s="71"/>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="B7" s="43"/>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="F8" s="10"/>
     </row>
   </sheetData>
@@ -5351,22 +5351,22 @@
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>134</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>2180.7671782733241</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>3260.9352996327957</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>2979.1279159518585</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>92</v>
       </c>
@@ -6379,14 +6379,14 @@
         <v>1848.0338796369435</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B7" s="42"/>
       <c r="C7" s="43"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B9" s="43"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B10" s="43"/>
     </row>
   </sheetData>
@@ -6407,23 +6407,23 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="9.1640625" style="1"/>
-    <col min="14" max="15" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="17.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="9.109375" style="1"/>
+    <col min="14" max="15" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>136</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
@@ -6777,10 +6777,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="43"/>
     </row>
@@ -6802,16 +6802,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Storage Volume [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Storage Volume [bbl]</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>117</v>
       </c>
@@ -6843,18 +6843,18 @@
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Pipeline Capacity between Sites [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>211</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
         <v>92</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="68" t="s">
         <v>109</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>124</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>125</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>126</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>127</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>128</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>129</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>130</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>131</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="68" t="s">
         <v>132</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="68" t="s">
         <v>117</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>14286</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>114</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>42857</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="68" t="s">
         <v>115</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>42857</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>119</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27" t="s">
         <v>120</v>
       </c>
@@ -7871,19 +7871,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Disposal Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>212</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>9285.7142857143008</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
@@ -7922,72 +7922,72 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="3.5" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.1640625" style="1"/>
-    <col min="13" max="13" width="11.1640625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="3.44140625" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="11.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="12.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.44140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
     </row>
   </sheetData>
@@ -8008,19 +8008,19 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Storage Capacity [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>117</v>
       </c>
@@ -8053,19 +8053,19 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="16.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Treatment Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
@@ -8106,13 +8106,13 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
@@ -8136,7 +8136,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>146</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>114</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>49999.999999999978</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>115</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>30000.000000000025</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
       <c r="F15" s="10"/>
     </row>
   </sheetData>
@@ -8744,19 +8744,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="11.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>212</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
@@ -8798,19 +8798,19 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Treatment Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -8818,7 +8818,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -8851,20 +8851,20 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pipeline Operational Cost between Sites [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>211</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
         <v>92</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="68" t="s">
         <v>109</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>124</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>125</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>126</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>127</v>
       </c>
@@ -9364,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>128</v>
       </c>
@@ -9414,7 +9414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>129</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>130</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>131</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="68" t="s">
         <v>132</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="68" t="s">
         <v>117</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>114</v>
       </c>
@@ -9714,7 +9714,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="68" t="s">
         <v>115</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>119</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27" t="s">
         <v>120</v>
       </c>
@@ -9882,14 +9882,14 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>117</v>
       </c>
@@ -9921,14 +9921,14 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>151</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>117</v>
       </c>
@@ -9957,22 +9957,22 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="19.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Souring Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>146</v>
       </c>
@@ -9980,7 +9980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>114</v>
       </c>
@@ -9988,7 +9988,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>115</v>
       </c>
@@ -10009,20 +10009,18 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Beneficial Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Beneficial Reuse Operational Cost [USD/bbl]</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10030,7 +10028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10038,7 +10036,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10059,40 +10057,40 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="3.5" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.1640625" style="1"/>
-    <col min="13" max="13" width="11.1640625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="3.44140625" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="11.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="12.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.44140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>97</v>
       </c>
@@ -10100,52 +10098,52 @@
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>107</v>
       </c>
@@ -10164,20 +10162,20 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Beneficial Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Beneficial Reuse Operational Cost [USD/bbl]</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10185,7 +10183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10193,7 +10191,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10215,18 +10213,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
         <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>211</v>
       </c>
@@ -10234,7 +10232,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -10242,7 +10240,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -10250,7 +10248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -10258,7 +10256,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
         <v>92</v>
       </c>
@@ -10266,7 +10264,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="85" t="s">
         <v>109</v>
       </c>
@@ -10274,7 +10272,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>114</v>
       </c>
@@ -10282,7 +10280,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
         <v>115</v>
       </c>
@@ -10306,17 +10304,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>211</v>
       </c>
@@ -10327,7 +10325,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>89</v>
       </c>
@@ -10338,7 +10336,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -10349,7 +10347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -10360,7 +10358,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
         <v>92</v>
       </c>
@@ -10371,7 +10369,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>109</v>
       </c>
@@ -10399,17 +10397,17 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10417,7 +10415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10425,7 +10423,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10449,17 +10447,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10470,7 +10468,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10481,7 +10479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10506,17 +10504,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>214</v>
       </c>
@@ -10524,7 +10522,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>121</v>
       </c>
@@ -10532,7 +10530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>122</v>
       </c>
@@ -10540,7 +10538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="79" t="s">
         <v>221</v>
       </c>
@@ -10548,7 +10546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
         <v>222</v>
       </c>
@@ -10556,7 +10554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>223</v>
       </c>
@@ -10578,17 +10576,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10596,7 +10594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10604,7 +10602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
@@ -10626,25 +10624,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>217</v>
       </c>
@@ -10655,7 +10653,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>89</v>
       </c>
@@ -10666,7 +10664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>90</v>
       </c>
@@ -10677,7 +10675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -10688,7 +10686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
         <v>92</v>
       </c>
@@ -10699,7 +10697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>109</v>
       </c>
@@ -10727,18 +10725,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [", VLOOKUP("concentration", Units!A2:B9, 2, FALSE),,"]")</f>
         <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>217</v>
       </c>
@@ -10749,7 +10747,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="88" t="s">
         <v>117</v>
       </c>
@@ -10774,14 +10772,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10789,7 +10787,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10797,7 +10795,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10819,36 +10817,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="3.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" style="1"/>
+    <col min="6" max="13" width="9.109375" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="11.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
     </row>
   </sheetData>
@@ -10866,14 +10864,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10884,7 +10882,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10895,7 +10893,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10919,14 +10917,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10937,7 +10935,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -10948,7 +10946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -10968,18 +10966,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E5B931-13ED-B04C-BD6B-B3248EDC4A69}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>148</v>
       </c>
@@ -10990,7 +10988,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -11001,7 +10999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>120</v>
       </c>
@@ -11026,38 +11024,38 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.1640625" style="1"/>
-    <col min="15" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.109375" style="1"/>
+    <col min="15" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
     </row>
   </sheetData>
@@ -11078,19 +11076,19 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -11108,33 +11106,33 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="3.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" style="1"/>
+    <col min="6" max="13" width="9.109375" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="11.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
added units for MinResidualQuality
</commit_message>
<xml_diff>
--- a/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
+++ b/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/models_extra/CM_module/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E94E631-B0AB-0342-B646-71961479F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EB1FC6-ABA7-9B44-B6AE-7382D3B8C05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5120" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="1" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="52" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -777,9 +777,6 @@
     <t>Li</t>
   </si>
   <si>
-    <t>Minimum Water Quality out of Residual Stream</t>
-  </si>
-  <si>
     <t>Choice on whether the site will treat that componenet or not</t>
   </si>
   <si>
@@ -799,6 +796,9 @@
   </si>
   <si>
     <t>Price earned based on each residuual treatment node [USD/bbl]</t>
+  </si>
+  <si>
+    <t>Minimum Water Quality out of Residual Stream [mg/L]</t>
   </si>
 </sst>
 </file>
@@ -4014,7 +4014,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4433,7 +4433,7 @@
   </sheetPr>
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -9864,7 +9864,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -9903,7 +9903,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -10754,7 +10754,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -10839,14 +10839,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -10891,15 +10891,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6983D6E2-EC48-E04B-A292-F019B326FE69}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -10944,7 +10942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E5B931-13ED-B04C-BD6B-B3248EDC4A69}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10952,7 +10950,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -11058,7 +11056,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correcting CM module case study headers (#318)
* correcting case study headers

* correcting links in headers of large permian cm case study

* added units for MinResidualQuality

---------

Co-authored-by: Travis Arnold <Travis.Arnold@netl.doe.gov>
</commit_message>
<xml_diff>
--- a/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
+++ b/pareto/models_extra/CM_module/case_studies/CM_small_permian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/case_studies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/models_extra/CM_module/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EA9594-653A-7E4B-A44B-503E8F484CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EB1FC6-ABA7-9B44-B6AE-7382D3B8C05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="52" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="52" activeTab="61" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -777,9 +777,6 @@
     <t>Li</t>
   </si>
   <si>
-    <t>Minimum Water Quality out of Residual Stream</t>
-  </si>
-  <si>
     <t>Choice on whether the site will treat that componenet or not</t>
   </si>
   <si>
@@ -799,6 +796,9 @@
   </si>
   <si>
     <t>Price earned based on each residuual treatment node [USD/bbl]</t>
+  </si>
+  <si>
+    <t>Minimum Water Quality out of Residual Stream [mg/L]</t>
   </si>
 </sst>
 </file>
@@ -4014,7 +4014,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4434,7 +4434,7 @@
   <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4982,9 +4982,7 @@
   </sheetPr>
   <dimension ref="A1:BC8"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
-    </sheetView>
+    <sheetView showZeros="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5347,9 +5345,7 @@
   </sheetPr>
   <dimension ref="A1:BA10"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6403,9 +6399,7 @@
   </sheetPr>
   <dimension ref="A1:BA6"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6839,9 +6833,7 @@
   </sheetPr>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
-    </sheetView>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7867,9 +7859,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8004,9 +7994,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8049,9 +8037,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8102,9 +8088,7 @@
   </sheetPr>
   <dimension ref="A1:BA15"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8740,9 +8724,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8794,9 +8776,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8847,9 +8827,7 @@
   </sheetPr>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9886,7 +9864,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -9925,7 +9903,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -9956,9 +9934,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10778,7 +10754,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -10863,14 +10839,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -10915,15 +10891,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6983D6E2-EC48-E04B-A292-F019B326FE69}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -10976,7 +10950,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -11082,7 +11056,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>